<commit_message>
replaced the sounding tables Renaming 'Classe 320' to 'HULL 320'
</commit_message>
<xml_diff>
--- a/library/Tabelas_Sondagem_SMIT_CARAJA.xlsx
+++ b/library/Tabelas_Sondagem_SMIT_CARAJA.xlsx
@@ -8,22 +8,23 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ÍNDICE" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AFTPEAK.C" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FF_FOAM.C" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FOREPEAK.C" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_AFT.P" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_AFT.S" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DAY.S" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.C" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.P" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.S" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_OF.P" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FRESH_WATER.P" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FRESH_WATER.S" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LUBE_OIL.S" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OILY_WTR.S" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SEWAGE.C" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WASTE_OIL.P" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DAY.P" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AFTPEAK.C" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FF_FOAM.C" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FOREPEAK.C" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_AFT.P" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_AFT.S" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DAY.S" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.C" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.P" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_DB.S" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FO_OF.P" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FRESH_WATER.P" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FRESH_WATER.S" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LUBE_OIL.S" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OILY_WTR.S" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SEWAGE.C" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WASTE_OIL.P" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -473,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,130 +582,142 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FO_DAY.S</t>
+          <t>FO_DAY.P</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tanque Diário de Óleo Combustível - Boreste</t>
+          <t>Tanque Diário de Óleo Combustível - Bombordo</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>FO_DB.C</t>
+          <t>FO_DAY.S</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tanque de Óleo Combustível Duplo Fundo - Centro</t>
+          <t>Tanque Diário de Óleo Combustível - Boreste</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>FO_DB.P</t>
+          <t>FO_DB.C</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Tanque de Óleo Combustível Duplo Fundo - Bombordo</t>
+          <t>Tanque de Óleo Combustível Duplo Fundo - Centro</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>FO_DB.S</t>
+          <t>FO_DB.P</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tanque de Óleo Combustível Duplo Fundo - Boreste</t>
+          <t>Tanque de Óleo Combustível Duplo Fundo - Bombordo</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FO_OF.P</t>
+          <t>FO_DB.S</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tanque de Overflow de Óleo Combustível - Bombordo</t>
+          <t>Tanque de Óleo Combustível Duplo Fundo - Boreste</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>FRESH_WATER.P</t>
+          <t>FO_OF.P</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tanque de Água Doce - Bombordo</t>
+          <t>Tanque de Overflow de Óleo Combustível - Bombordo</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FRESH_WATER.S</t>
+          <t>FRESH_WATER.P</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tanque de Água Doce - Boreste</t>
+          <t>Tanque de Água Doce - Bombordo</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LUBE_OIL.S</t>
+          <t>FRESH_WATER.S</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tanque de Óleo Lubrificante - Boreste</t>
+          <t>Tanque de Água Doce - Boreste</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>OILY_WTR.S</t>
+          <t>LUBE_OIL.S</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tanque de Água Oleosa - Boreste</t>
+          <t>Tanque de Óleo Lubrificante - Boreste</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SEWAGE.C</t>
+          <t>OILY_WTR.S</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tanque de Esgoto - Centro</t>
+          <t>Tanque de Água Oleosa - Boreste</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>SEWAGE.C</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Tanque de Esgoto - Centro</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>WASTE_OIL.P</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>Tanque de Óleo Residual - Bombordo</t>
         </is>
@@ -736,14 +749,14 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>TABELA: FO_DB.S</t>
+          <t>TABELA: FO_DB.P</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tanque de Óleo Combustível Duplo Fundo - Boreste</t>
+          <t>Tanque de Óleo Combustível Duplo Fundo - Bombordo</t>
         </is>
       </c>
     </row>
@@ -810,7 +823,7 @@
         <v>400</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>1761</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="12">
@@ -818,7 +831,7 @@
         <v>500</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>2703</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="13">
@@ -826,7 +839,7 @@
         <v>600</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>3859</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="14">
@@ -834,7 +847,7 @@
         <v>700</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>5170</v>
+        <v>5010</v>
       </c>
     </row>
     <row r="15">
@@ -842,7 +855,7 @@
         <v>800</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>6591</v>
+        <v>6308</v>
       </c>
     </row>
     <row r="16">
@@ -850,7 +863,7 @@
         <v>900</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>8102</v>
+        <v>7660</v>
       </c>
     </row>
     <row r="17">
@@ -858,7 +871,7 @@
         <v>1000</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>9683</v>
+        <v>9053</v>
       </c>
     </row>
     <row r="18">
@@ -866,7 +879,7 @@
         <v>1100</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>11321</v>
+        <v>10479</v>
       </c>
     </row>
     <row r="19">
@@ -874,7 +887,7 @@
         <v>1200</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>13004</v>
+        <v>11937</v>
       </c>
     </row>
     <row r="20">
@@ -882,7 +895,7 @@
         <v>1300</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>14728</v>
+        <v>13427</v>
       </c>
     </row>
     <row r="21">
@@ -890,7 +903,7 @@
         <v>1400</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>16492</v>
+        <v>14948</v>
       </c>
     </row>
     <row r="22">
@@ -898,7 +911,7 @@
         <v>1500</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>18295</v>
+        <v>16499</v>
       </c>
     </row>
     <row r="23">
@@ -906,7 +919,7 @@
         <v>1600</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>20125</v>
+        <v>18071</v>
       </c>
     </row>
     <row r="24">
@@ -914,7 +927,7 @@
         <v>1700</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>22040</v>
+        <v>19710</v>
       </c>
     </row>
     <row r="25">
@@ -922,7 +935,7 @@
         <v>1800</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>24222</v>
+        <v>21593</v>
       </c>
     </row>
     <row r="26">
@@ -930,7 +943,7 @@
         <v>1900</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>26643</v>
+        <v>23711</v>
       </c>
     </row>
     <row r="27">
@@ -938,7 +951,7 @@
         <v>2000</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>29225</v>
+        <v>25966</v>
       </c>
     </row>
     <row r="28">
@@ -946,15 +959,15 @@
         <v>2100</v>
       </c>
       <c r="B28" s="5" t="n">
-        <v>31904</v>
+        <v>28304</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="n">
-        <v>2200</v>
+        <v>2182</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>34110</v>
+        <v>30231</v>
       </c>
     </row>
     <row r="30">
@@ -964,7 +977,7 @@
         </is>
       </c>
       <c r="B30" s="6" t="n">
-        <v>34110</v>
+        <v>30231</v>
       </c>
     </row>
   </sheetData>
@@ -973,6 +986,263 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>TABELA: FO_DB.S</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tanque de Óleo Combustível Duplo Fundo - Boreste</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SMIT CARAJÁ (HULL 326) - Ramparts 3000 Tug</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Robert Allan Ltd | No Trim, No Heel</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Sondagem (mm)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Volume (litros)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n">
+        <v>400</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>3859</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="n">
+        <v>700</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>5170</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>6591</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>8102</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>9683</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>11321</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>13004</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>14728</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>16492</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>18295</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n">
+        <v>1600</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>20125</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n">
+        <v>1700</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>22040</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>24222</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n">
+        <v>1900</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>26643</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>29225</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n">
+        <v>2100</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>31904</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n">
+        <v>2200</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>34110</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>CAPACIDADE TOTAL:</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>34110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1206,447 +1476,6 @@
       </c>
       <c r="B28" s="6" t="n">
         <v>3533</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>TABELA: FRESH_WATER.P</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tanque de Água Doce - Bombordo</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SMIT CARAJÁ (HULL 326) - Ramparts 3000 Tug</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Robert Allan Ltd | No Trim, No Heel</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Sondagem (mm)</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Volume (litros)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="n">
-        <v>200</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="n">
-        <v>400</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="n">
-        <v>600</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n">
-        <v>700</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n">
-        <v>800</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="n">
-        <v>900</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B17" s="5" t="n">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="n">
-        <v>1100</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="B19" s="5" t="n">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="B20" s="5" t="n">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="n">
-        <v>1400</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="B22" s="5" t="n">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="n">
-        <v>1600</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="n">
-        <v>1700</v>
-      </c>
-      <c r="B24" s="5" t="n">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="n">
-        <v>1800</v>
-      </c>
-      <c r="B25" s="5" t="n">
-        <v>1706</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="n">
-        <v>1900</v>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="B27" s="5" t="n">
-        <v>2330</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="n">
-        <v>2100</v>
-      </c>
-      <c r="B28" s="5" t="n">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="n">
-        <v>2200</v>
-      </c>
-      <c r="B29" s="5" t="n">
-        <v>3014</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="n">
-        <v>2300</v>
-      </c>
-      <c r="B30" s="5" t="n">
-        <v>3378</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="5" t="n">
-        <v>2400</v>
-      </c>
-      <c r="B31" s="5" t="n">
-        <v>3755</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="n">
-        <v>2500</v>
-      </c>
-      <c r="B32" s="5" t="n">
-        <v>4143</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="n">
-        <v>2600</v>
-      </c>
-      <c r="B33" s="5" t="n">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="5" t="n">
-        <v>2700</v>
-      </c>
-      <c r="B34" s="5" t="n">
-        <v>4946</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="5" t="n">
-        <v>2800</v>
-      </c>
-      <c r="B35" s="5" t="n">
-        <v>5359</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="5" t="n">
-        <v>2900</v>
-      </c>
-      <c r="B36" s="5" t="n">
-        <v>5778</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="B37" s="5" t="n">
-        <v>6205</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="5" t="n">
-        <v>3100</v>
-      </c>
-      <c r="B38" s="5" t="n">
-        <v>6638</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="5" t="n">
-        <v>3200</v>
-      </c>
-      <c r="B39" s="5" t="n">
-        <v>7078</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="5" t="n">
-        <v>3300</v>
-      </c>
-      <c r="B40" s="5" t="n">
-        <v>7524</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="5" t="n">
-        <v>3400</v>
-      </c>
-      <c r="B41" s="5" t="n">
-        <v>7977</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="5" t="n">
-        <v>3500</v>
-      </c>
-      <c r="B42" s="5" t="n">
-        <v>8436</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="5" t="n">
-        <v>3600</v>
-      </c>
-      <c r="B43" s="5" t="n">
-        <v>8901</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="5" t="n">
-        <v>3700</v>
-      </c>
-      <c r="B44" s="5" t="n">
-        <v>9373</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="5" t="n">
-        <v>3800</v>
-      </c>
-      <c r="B45" s="5" t="n">
-        <v>9866</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="5" t="n">
-        <v>3900</v>
-      </c>
-      <c r="B46" s="5" t="n">
-        <v>10392</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="5" t="n">
-        <v>4000</v>
-      </c>
-      <c r="B47" s="5" t="n">
-        <v>10942</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="5" t="n">
-        <v>4100</v>
-      </c>
-      <c r="B48" s="5" t="n">
-        <v>11507</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="5" t="n">
-        <v>4200</v>
-      </c>
-      <c r="B49" s="5" t="n">
-        <v>12081</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="5" t="n">
-        <v>4300</v>
-      </c>
-      <c r="B50" s="5" t="n">
-        <v>12661</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="5" t="n">
-        <v>4400</v>
-      </c>
-      <c r="B51" s="5" t="n">
-        <v>13248</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="5" t="n">
-        <v>4448</v>
-      </c>
-      <c r="B52" s="5" t="n">
-        <v>13520</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="6" t="inlineStr">
-        <is>
-          <t>CAPACIDADE TOTAL:</t>
-        </is>
-      </c>
-      <c r="B53" s="6" t="n">
-        <v>13520</v>
       </c>
     </row>
   </sheetData>
@@ -1675,14 +1504,14 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>TABELA: FRESH_WATER.S</t>
+          <t>TABELA: FRESH_WATER.P</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tanque de Água Doce - Boreste</t>
+          <t>Tanque de Água Doce - Bombordo</t>
         </is>
       </c>
     </row>
@@ -2096,6 +1925,447 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>TABELA: FRESH_WATER.S</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tanque de Água Doce - Boreste</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SMIT CARAJÁ (HULL 326) - Ramparts 3000 Tug</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Robert Allan Ltd | No Trim, No Heel</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Sondagem (mm)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Volume (litros)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n">
+        <v>400</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="n">
+        <v>700</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n">
+        <v>1600</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n">
+        <v>1700</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n">
+        <v>1900</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n">
+        <v>2100</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n">
+        <v>2200</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="n">
+        <v>2300</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>3378</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>4143</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="n">
+        <v>2600</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="n">
+        <v>2700</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>4946</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="n">
+        <v>2800</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>5359</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="n">
+        <v>2900</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>5778</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="n">
+        <v>3100</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>6638</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="n">
+        <v>3200</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>7078</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="n">
+        <v>3300</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>7524</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="n">
+        <v>3400</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>7977</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="5" t="n">
+        <v>3500</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>8436</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="n">
+        <v>3600</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>8901</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="n">
+        <v>3700</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>9373</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="n">
+        <v>3800</v>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>9866</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="5" t="n">
+        <v>3900</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>10392</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="5" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B47" s="5" t="n">
+        <v>10942</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="5" t="n">
+        <v>4100</v>
+      </c>
+      <c r="B48" s="5" t="n">
+        <v>11507</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="n">
+        <v>4200</v>
+      </c>
+      <c r="B49" s="5" t="n">
+        <v>12081</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="5" t="n">
+        <v>4300</v>
+      </c>
+      <c r="B50" s="5" t="n">
+        <v>12661</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="5" t="n">
+        <v>4400</v>
+      </c>
+      <c r="B51" s="5" t="n">
+        <v>13248</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="n">
+        <v>4448</v>
+      </c>
+      <c r="B52" s="5" t="n">
+        <v>13520</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>CAPACIDADE TOTAL:</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="n">
+        <v>13520</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2336,7 +2606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2609,7 +2879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2842,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3097,6 +3367,319 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>TABELA: FO_DAY.P</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tanque Diário de Óleo Combustível - Bombordo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SMIT CARAJÁ (HULL 326) - Ramparts 3000 Tug</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Robert Allan Ltd | No Trim, No Heel</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Sondagem (mm)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Volume (litros)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n">
+        <v>400</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>4816</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="n">
+        <v>700</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>5603</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>6392</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>7182</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>7975</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>8769</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>9565</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>10363</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>11162</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>11964</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n">
+        <v>1600</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>12767</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n">
+        <v>1700</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>13572</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>14379</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n">
+        <v>1900</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>15187</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>15998</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n">
+        <v>2100</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>16810</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n">
+        <v>2200</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>17623</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="n">
+        <v>2300</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>18436</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>19249</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>20062</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="n">
+        <v>2600</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>20875</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="n">
+        <v>2700</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>21688</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="n">
+        <v>2800</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>22491</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="n">
+        <v>2848</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>22623</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>CAPACIDADE TOTAL:</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>22623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3444,7 +4027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3677,7 +4260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4238,7 +4821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4503,7 +5086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4784,7 +5367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5097,7 +5680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5368,261 +5951,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>TABELA: FO_DB.P</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tanque de Óleo Combustível Duplo Fundo - Bombordo</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SMIT CARAJÁ (HULL 326) - Ramparts 3000 Tug</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Robert Allan Ltd | No Trim, No Heel</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Sondagem (mm)</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Volume (litros)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="n">
-        <v>200</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="n">
-        <v>400</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>2676</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="n">
-        <v>600</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>3784</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n">
-        <v>700</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>5010</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n">
-        <v>800</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>6308</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="n">
-        <v>900</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>7660</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B17" s="5" t="n">
-        <v>9053</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="n">
-        <v>1100</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>10479</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="B19" s="5" t="n">
-        <v>11937</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="B20" s="5" t="n">
-        <v>13427</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="n">
-        <v>1400</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>14948</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="B22" s="5" t="n">
-        <v>16499</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="n">
-        <v>1600</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <v>18071</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="n">
-        <v>1700</v>
-      </c>
-      <c r="B24" s="5" t="n">
-        <v>19710</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="n">
-        <v>1800</v>
-      </c>
-      <c r="B25" s="5" t="n">
-        <v>21593</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="n">
-        <v>1900</v>
-      </c>
-      <c r="B26" s="5" t="n">
-        <v>23711</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="B27" s="5" t="n">
-        <v>25966</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="n">
-        <v>2100</v>
-      </c>
-      <c r="B28" s="5" t="n">
-        <v>28304</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="n">
-        <v>2182</v>
-      </c>
-      <c r="B29" s="5" t="n">
-        <v>30231</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="inlineStr">
-        <is>
-          <t>CAPACIDADE TOTAL:</t>
-        </is>
-      </c>
-      <c r="B30" s="6" t="n">
-        <v>30231</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>